<commit_message>
Add move and turn
</commit_message>
<xml_diff>
--- a/00_task/psp.xlsx
+++ b/00_task/psp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zholu\Documents\Programming\cleanarch\00_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D508EE-3BAE-4B07-AB49-E81E1224CF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66020472-D88D-450F-8BD2-B867A2DC21F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{92739D6D-7919-4FB4-9076-00A3E99E5C9B}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Планирование</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Непродуманная система типов</t>
+  </si>
+  <si>
+    <t>ребёнок</t>
+  </si>
+  <si>
+    <t>ScrollLock</t>
   </si>
 </sst>
 </file>
@@ -783,10 +789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B38188-8D4C-479A-BEB8-B60DCCD00AF4}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,6 +888,37 @@
       </c>
       <c r="C13" s="2">
         <v>0.34166666666666662</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <v>0.37986111111111115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <v>0.38125000000000003</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <v>0.3840277777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>